<commit_message>
Changes webpages en structuur
</commit_message>
<xml_diff>
--- a/Status Standaardenregister.xlsx
+++ b/Status Standaardenregister.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="40">
   <si>
     <t>Standaard</t>
   </si>
@@ -36,9 +36,6 @@
     <t>Html</t>
   </si>
   <si>
-    <t>Documenten</t>
-  </si>
-  <si>
     <t>Erkende Standaard</t>
   </si>
   <si>
@@ -112,16 +109,62 @@
   </si>
   <si>
     <t>Vocabularium Transactie</t>
+  </si>
+  <si>
+    <t>Datastandaarden Register</t>
+  </si>
+  <si>
+    <t>Content</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Review intro needed 
+Quid links to Standards</t>
+  </si>
+  <si>
+    <t>Links TBD</t>
+  </si>
+  <si>
+    <t>OSLO Datastandaardenregister webpage</t>
+  </si>
+  <si>
+    <t>Only drafts?</t>
+  </si>
+  <si>
+    <t>Available documentation</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Webcast 4/5
+Thematische WG</t>
+  </si>
+  <si>
+    <t>Specs?</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/drive/u/2/folders/0B5lYzh34rTaucXo3Slc1alV4eWc</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -144,10 +187,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -161,11 +205,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="7">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -195,13 +258,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="C4:F25" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="C4:F25"/>
-  <tableColumns count="4">
-    <tableColumn id="1" name="Categorie" dataDxfId="3"/>
-    <tableColumn id="2" name="Standaard" dataDxfId="2"/>
-    <tableColumn id="3" name="Html" dataDxfId="1"/>
-    <tableColumn id="4" name="Documenten" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A4:F26" totalsRowShown="0" headerRowDxfId="6">
+  <autoFilter ref="A4:F26"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Categorie" dataDxfId="5"/>
+    <tableColumn id="2" name="Standaard" dataDxfId="4"/>
+    <tableColumn id="3" name="Html" dataDxfId="3"/>
+    <tableColumn id="4" name="Content" dataDxfId="2"/>
+    <tableColumn id="6" name="Available documentation" dataDxfId="1"/>
+    <tableColumn id="5" name="Comments" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -488,260 +553,345 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:F25"/>
+  <dimension ref="A3:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="29.25" customWidth="1"/>
-    <col min="2" max="2" width="27.5" customWidth="1"/>
-    <col min="3" max="3" width="24.75" customWidth="1"/>
-    <col min="4" max="4" width="42.25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.375" customWidth="1"/>
-    <col min="6" max="6" width="36" customWidth="1"/>
+    <col min="1" max="1" width="24.75" customWidth="1"/>
+    <col min="2" max="2" width="42.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.375" customWidth="1"/>
+    <col min="4" max="5" width="36" customWidth="1"/>
+    <col min="6" max="6" width="27.25" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-    </row>
-    <row r="4" spans="3:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>0</v>
+      </c>
       <c r="C4" s="3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="3:6" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>33</v>
+      </c>
       <c r="C5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="5"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="5"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="5"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="5"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="5"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="5"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="5"/>
+    </row>
+    <row r="15" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-    </row>
-    <row r="6" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C6" s="1" t="s">
+      <c r="B17" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="5"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-    </row>
-    <row r="7" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C7" s="1" t="s">
+      <c r="B18" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="5"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-    </row>
-    <row r="8" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C8" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-    </row>
-    <row r="9" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C9" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F9" s="1"/>
-    </row>
-    <row r="10" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C10" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-    </row>
-    <row r="11" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C11" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-    </row>
-    <row r="12" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C12" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-    </row>
-    <row r="13" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C13" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-    </row>
-    <row r="14" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C14" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-    </row>
-    <row r="15" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C15" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-    </row>
-    <row r="16" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C16" s="1" t="s">
+      <c r="B19" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="5"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D16" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-    </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C17" s="1" t="s">
+      <c r="B20" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="5"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D17" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F17" s="1"/>
-    </row>
-    <row r="18" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C18" s="1" t="s">
+      <c r="B21" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="5"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D18" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-    </row>
-    <row r="19" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C19" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-    </row>
-    <row r="20" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C20" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D20" s="4" t="s">
+      <c r="B22" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-    </row>
-    <row r="21" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C21" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D21" s="4" t="s">
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="5"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-    </row>
-    <row r="22" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C22" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D22" s="4" t="s">
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="5"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-    </row>
-    <row r="23" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C23" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D23" s="4" t="s">
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="5"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-    </row>
-    <row r="24" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C24" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D24" s="4" t="s">
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="5"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-    </row>
-    <row r="25" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C25" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="5"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F15" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
@@ -750,7 +900,7 @@
           <x14:formula1>
             <xm:f>Sheet2!$A$1:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>C5:C53</xm:sqref>
+          <xm:sqref>A6:A54</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -770,17 +920,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>